<commit_message>
Add GA solution files and GAinfo.txt. Added new selection and mutation methods for GA.
</commit_message>
<xml_diff>
--- a/TSP/Solver_solutions/Dane_TSP_76_rozw_solver.xlsx
+++ b/TSP/Solver_solutions/Dane_TSP_76_rozw_solver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\Programowanie\ComputationalInteligence\TSP\Solver_solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitProjects\ComputationalInteligence\TSP\Solver_solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9755AEDF-D1E8-4DF5-83D0-F4CB13939C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC746667-CEBA-42A9-B8E5-EF337B605AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{2E92C40E-D2D6-4D6C-8826-671A9922C679}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E92C40E-D2D6-4D6C-8826-671A9922C679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="solver_adj" localSheetId="0" hidden="1">Arkusz1!$B$80:$B$155</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Arkusz1!$B$80:$B$155</definedName>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -487,12 +487,12 @@
   <dimension ref="A1:BY156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+      <selection activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
@@ -722,7 +722,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -955,7 +955,7 @@
         <v>3716.180835212409</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>3828.8379438153288</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>6689.7309362933274</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>7179.3105518566344</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>8305.0751351206927</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>7625.2903551274694</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>7027.2683170631817</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>7071.9516401061464</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>8875.3873154922094</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>9250</v>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>10718.49378410978</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>10199.057211330861</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>10562.196741208711</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>10556.15933945675</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>11746.169588423279</v>
       </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>12031.728886573201</v>
       </c>
     </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>11899.684869777009</v>
       </c>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>12386.787315522941</v>
       </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>9592.3146320374617</v>
       </c>
     </row>
-    <row r="21" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>8912.0704665077683</v>
       </c>
     </row>
-    <row r="22" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>7527.2837066235252</v>
       </c>
     </row>
-    <row r="23" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>6622.1220163932348</v>
       </c>
     </row>
-    <row r="24" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>5261.1785751863617</v>
       </c>
     </row>
-    <row r="25" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>8286.8872322483057</v>
       </c>
     </row>
-    <row r="26" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>8048.1364302551428</v>
       </c>
     </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>10491.186777481371</v>
       </c>
     </row>
-    <row r="28" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>11113.28034380488</v>
       </c>
     </row>
-    <row r="29" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>11954.613042671021</v>
       </c>
     </row>
-    <row r="30" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>11022.297990891009</v>
       </c>
     </row>
-    <row r="31" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>10210.0440743417</v>
       </c>
     </row>
-    <row r="32" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>10006.248048094751</v>
       </c>
     </row>
-    <row r="33" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>12003.54114417908</v>
       </c>
     </row>
-    <row r="34" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>12550.896382330629</v>
       </c>
     </row>
-    <row r="35" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8644,7 +8644,7 @@
         <v>13742.038022069361</v>
       </c>
     </row>
-    <row r="36" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8877,7 +8877,7 @@
         <v>12936.663712101359</v>
       </c>
     </row>
-    <row r="37" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9110,7 +9110,7 @@
         <v>12900.48448702606</v>
       </c>
     </row>
-    <row r="38" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>12710.03540514345</v>
       </c>
     </row>
-    <row r="39" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9576,7 +9576,7 @@
         <v>14257.804880134951</v>
       </c>
     </row>
-    <row r="40" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9809,7 +9809,7 @@
         <v>14721.58279533828</v>
       </c>
     </row>
-    <row r="41" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>15014.65950329877</v>
       </c>
     </row>
-    <row r="42" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10275,7 +10275,7 @@
         <v>15602.72412112705</v>
       </c>
     </row>
-    <row r="43" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10508,7 +10508,7 @@
         <v>13491.664093061319</v>
       </c>
     </row>
-    <row r="44" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10741,7 +10741,7 @@
         <v>12777.421492617361</v>
       </c>
     </row>
-    <row r="45" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10974,7 +10974,7 @@
         <v>12110.842249818959</v>
       </c>
     </row>
-    <row r="46" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11207,7 +11207,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="47" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>9982.1089955980751</v>
       </c>
     </row>
-    <row r="48" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11673,7 +11673,7 @@
         <v>12986.916493148021</v>
       </c>
     </row>
-    <row r="49" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11906,7 +11906,7 @@
         <v>12649.50591920491</v>
       </c>
     </row>
-    <row r="50" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -12139,7 +12139,7 @@
         <v>14849.32658405761</v>
       </c>
     </row>
-    <row r="51" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -12372,7 +12372,7 @@
         <v>15511.044452260459</v>
       </c>
     </row>
-    <row r="52" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -12605,7 +12605,7 @@
         <v>16185.681110166481</v>
       </c>
     </row>
-    <row r="53" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -12838,7 +12838,7 @@
         <v>15164.499760954861</v>
       </c>
     </row>
-    <row r="54" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -13071,7 +13071,7 @@
         <v>14290.99366734168</v>
       </c>
     </row>
-    <row r="55" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -13304,7 +13304,7 @@
         <v>13977.213599283659</v>
       </c>
     </row>
-    <row r="56" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13537,7 +13537,7 @@
         <v>15953.7613119916</v>
       </c>
     </row>
-    <row r="57" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -13770,7 +13770,7 @@
         <v>16571.43626847112</v>
       </c>
     </row>
-    <row r="58" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -14003,7 +14003,7 @@
         <v>17547.823483269942</v>
       </c>
     </row>
-    <row r="59" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -14236,7 +14236,7 @@
         <v>16607.79238791237</v>
       </c>
     </row>
-    <row r="60" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -14469,7 +14469,7 @@
         <v>16322.07094703365</v>
       </c>
     </row>
-    <row r="61" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -14702,7 +14702,7 @@
         <v>16024.434467400089</v>
       </c>
     </row>
-    <row r="62" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -14935,7 +14935,7 @@
         <v>17712.213300431991</v>
       </c>
     </row>
-    <row r="63" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>18270.536390593461</v>
       </c>
     </row>
-    <row r="64" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -15401,7 +15401,7 @@
         <v>18825.58100033037</v>
       </c>
     </row>
-    <row r="65" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>19457.196612050771</v>
       </c>
     </row>
-    <row r="66" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -15867,7 +15867,7 @@
         <v>17809.05668473207</v>
       </c>
     </row>
-    <row r="67" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -16100,7 +16100,7 @@
         <v>17094.5897874152</v>
       </c>
     </row>
-    <row r="68" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -16333,7 +16333,7 @@
         <v>16787.197502859141</v>
       </c>
     </row>
-    <row r="69" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -16566,7 +16566,7 @@
         <v>16020.37764848257</v>
       </c>
     </row>
-    <row r="70" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -16799,7 +16799,7 @@
         <v>14721.75261305528</v>
       </c>
     </row>
-    <row r="71" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -17032,7 +17032,7 @@
         <v>19600</v>
       </c>
     </row>
-    <row r="72" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -17265,7 +17265,7 @@
         <v>21651.789764358971</v>
       </c>
     </row>
-    <row r="73" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -17498,7 +17498,7 @@
         <v>22524.87513838867</v>
       </c>
     </row>
-    <row r="74" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -17731,7 +17731,7 @@
         <v>22674.214429611449</v>
       </c>
     </row>
-    <row r="75" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -17964,7 +17964,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="76" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -18197,7 +18197,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="77" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -18430,7 +18430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -18441,925 +18441,925 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>1</v>
       </c>
       <c r="B80" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C80" s="1" cm="1">
         <f t="array" ref="C80">INDEX($B$2:$BY$77,B80,B81)</f>
-        <v>3716.180835212409</v>
+        <v>905.84380552057644</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>2</v>
       </c>
       <c r="B81" s="2">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C81" s="1" cm="1">
         <f t="array" ref="C81">INDEX($B$2:$BY$77,B81,B82)</f>
-        <v>3828.8379438153288</v>
+        <v>1115.0004484304029</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>3</v>
       </c>
       <c r="B82" s="2">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C82" s="1" cm="1">
         <f t="array" ref="C82">INDEX($B$2:$BY$77,B82,B83)</f>
-        <v>2926.1749776799061</v>
+        <v>1362.9647831107011</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>4</v>
       </c>
       <c r="B83" s="2">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C83" s="1" cm="1">
         <f t="array" ref="C83">INDEX($B$2:$BY$77,B83,B84)</f>
         <v>700</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>5</v>
       </c>
       <c r="B84" s="2">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C84" s="1" cm="1">
         <f t="array" ref="C84">INDEX($B$2:$BY$77,B84,B85)</f>
-        <v>1368.89480969138</v>
+        <v>1615.446687452112</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>6</v>
       </c>
       <c r="B85" s="2">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C85" s="1" cm="1">
         <f t="array" ref="C85">INDEX($B$2:$BY$77,B85,B86)</f>
-        <v>1115.0004484304029</v>
+        <v>2139.571919800781</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>7</v>
       </c>
       <c r="B86" s="2">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C86" s="1" cm="1">
         <f t="array" ref="C86">INDEX($B$2:$BY$77,B86,B87)</f>
-        <v>905.84380552057644</v>
+        <v>667.08320320631674</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>8</v>
       </c>
       <c r="B87" s="2">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C87" s="1" cm="1">
         <f t="array" ref="C87">INDEX($B$2:$BY$77,B87,B88)</f>
-        <v>583.09518948453001</v>
+        <v>1511.6216457830969</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>9</v>
       </c>
       <c r="B88" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C88" s="1" cm="1">
         <f t="array" ref="C88">INDEX($B$2:$BY$77,B88,B89)</f>
-        <v>2000</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>10</v>
       </c>
       <c r="B89" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C89" s="1" cm="1">
         <f t="array" ref="C89">INDEX($B$2:$BY$77,B89,B90)</f>
-        <v>700</v>
+        <v>4533.4865170197654</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>11</v>
       </c>
       <c r="B90" s="2">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C90" s="1" cm="1">
         <f t="array" ref="C90">INDEX($B$2:$BY$77,B90,B91)</f>
-        <v>1616.696941297286</v>
+        <v>3157.9265349276261</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>12</v>
       </c>
       <c r="B91" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C91" s="1" cm="1">
         <f t="array" ref="C91">INDEX($B$2:$BY$77,B91,B92)</f>
-        <v>1118.0004472271021</v>
+        <v>522.01532544552754</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>13</v>
       </c>
       <c r="B92" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C92" s="1" cm="1">
         <f t="array" ref="C92">INDEX($B$2:$BY$77,B92,B93)</f>
         <v>1164.11683262463</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>14</v>
       </c>
       <c r="B93" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C93" s="1" cm="1">
         <f t="array" ref="C93">INDEX($B$2:$BY$77,B93,B94)</f>
-        <v>522.01532544552754</v>
+        <v>1615.446687452112</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>15</v>
       </c>
       <c r="B94" s="2">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C94" s="1" cm="1">
         <f t="array" ref="C94">INDEX($B$2:$BY$77,B94,B95)</f>
-        <v>1746.424919657298</v>
+        <v>1363.8009385537171</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>16</v>
       </c>
       <c r="B95" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C95" s="1" cm="1">
         <f t="array" ref="C95">INDEX($B$2:$BY$77,B95,B96)</f>
-        <v>700</v>
+        <v>1115.0004484304029</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>17</v>
       </c>
       <c r="B96" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C96" s="1" cm="1">
         <f t="array" ref="C96">INDEX($B$2:$BY$77,B96,B97)</f>
-        <v>1511.6216457830969</v>
+        <v>1368.89480969138</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>18</v>
       </c>
       <c r="B97" s="2">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C97" s="1" cm="1">
         <f t="array" ref="C97">INDEX($B$2:$BY$77,B97,B98)</f>
-        <v>667.08320320631674</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>19</v>
       </c>
       <c r="B98" s="2">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C98" s="1" cm="1">
         <f t="array" ref="C98">INDEX($B$2:$BY$77,B98,B99)</f>
-        <v>3700</v>
+        <v>1627.8820596099711</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>20</v>
       </c>
       <c r="B99" s="2">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C99" s="1" cm="1">
         <f t="array" ref="C99">INDEX($B$2:$BY$77,B99,B100)</f>
-        <v>715.89105316381767</v>
+        <v>583.09518948453001</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>21</v>
       </c>
       <c r="B100" s="2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C100" s="1" cm="1">
         <f t="array" ref="C100">INDEX($B$2:$BY$77,B100,B101)</f>
-        <v>3707.4249823833252</v>
+        <v>3950</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>22</v>
       </c>
       <c r="B101" s="2">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C101" s="1" cm="1">
         <f t="array" ref="C101">INDEX($B$2:$BY$77,B101,B102)</f>
-        <v>1192.6860441876561</v>
+        <v>3828.8379438153288</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>23</v>
       </c>
       <c r="B102" s="2">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="C102" s="1" cm="1">
         <f t="array" ref="C102">INDEX($B$2:$BY$77,B102,B103)</f>
-        <v>1432.6548781894401</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>24</v>
       </c>
       <c r="B103" s="2">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C103" s="1" cm="1">
         <f t="array" ref="C103">INDEX($B$2:$BY$77,B103,B104)</f>
-        <v>3031.913587159107</v>
+        <v>3605.551275463989</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>25</v>
       </c>
       <c r="B104" s="2">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C104" s="1" cm="1">
         <f t="array" ref="C104">INDEX($B$2:$BY$77,B104,B105)</f>
-        <v>1118.0339887498949</v>
+        <v>1931.320791582797</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>26</v>
       </c>
       <c r="B105" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C105" s="1" cm="1">
         <f t="array" ref="C105">INDEX($B$2:$BY$77,B105,B106)</f>
-        <v>2926.1749776799061</v>
+        <v>1432.6548781894401</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>27</v>
       </c>
       <c r="B106" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C106" s="1" cm="1">
         <f t="array" ref="C106">INDEX($B$2:$BY$77,B106,B107)</f>
-        <v>700</v>
+        <v>1700</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>28</v>
       </c>
       <c r="B107" s="2">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C107" s="1" cm="1">
         <f t="array" ref="C107">INDEX($B$2:$BY$77,B107,B108)</f>
-        <v>1368.89480969138</v>
+        <v>1450</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>29</v>
       </c>
       <c r="B108" s="2">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C108" s="1" cm="1">
         <f t="array" ref="C108">INDEX($B$2:$BY$77,B108,B109)</f>
-        <v>1115.0004484304029</v>
+        <v>550</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>30</v>
       </c>
       <c r="B109" s="2">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C109" s="1" cm="1">
         <f t="array" ref="C109">INDEX($B$2:$BY$77,B109,B110)</f>
-        <v>905.84380552057644</v>
+        <v>2926.1749776799061</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>31</v>
       </c>
       <c r="B110" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C110" s="1" cm="1">
         <f t="array" ref="C110">INDEX($B$2:$BY$77,B110,B111)</f>
-        <v>583.09518948453001</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>32</v>
       </c>
       <c r="B111" s="2">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C111" s="1" cm="1">
         <f t="array" ref="C111">INDEX($B$2:$BY$77,B111,B112)</f>
-        <v>2000</v>
+        <v>4150</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>33</v>
       </c>
       <c r="B112" s="2">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C112" s="1" cm="1">
         <f t="array" ref="C112">INDEX($B$2:$BY$77,B112,B113)</f>
-        <v>700</v>
+        <v>1432.6548781894401</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>34</v>
       </c>
       <c r="B113" s="2">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C113" s="1" cm="1">
         <f t="array" ref="C113">INDEX($B$2:$BY$77,B113,B114)</f>
-        <v>1616.696941297286</v>
+        <v>1192.6860441876561</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>35</v>
       </c>
       <c r="B114" s="2">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C114" s="1" cm="1">
         <f t="array" ref="C114">INDEX($B$2:$BY$77,B114,B115)</f>
-        <v>1118.0004472271021</v>
+        <v>550</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>36</v>
       </c>
       <c r="B115" s="2">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C115" s="1" cm="1">
         <f t="array" ref="C115">INDEX($B$2:$BY$77,B115,B116)</f>
-        <v>1164.11683262463</v>
+        <v>1118.0339887498949</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>37</v>
       </c>
       <c r="B116" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C116" s="1" cm="1">
         <f t="array" ref="C116">INDEX($B$2:$BY$77,B116,B117)</f>
-        <v>522.01532544552754</v>
+        <v>1931.320791582797</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>38</v>
       </c>
       <c r="B117" s="2">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C117" s="1" cm="1">
         <f t="array" ref="C117">INDEX($B$2:$BY$77,B117,B118)</f>
-        <v>1746.424919657298</v>
+        <v>1432.6548781894401</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>39</v>
       </c>
       <c r="B118" s="2">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C118" s="1" cm="1">
         <f t="array" ref="C118">INDEX($B$2:$BY$77,B118,B119)</f>
-        <v>700</v>
+        <v>3946.200704475129</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>40</v>
       </c>
       <c r="B119" s="2">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C119" s="1" cm="1">
         <f t="array" ref="C119">INDEX($B$2:$BY$77,B119,B120)</f>
-        <v>1511.6216457830969</v>
+        <v>3905.1248379533272</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>41</v>
       </c>
       <c r="B120" s="2">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C120" s="1" cm="1">
         <f t="array" ref="C120">INDEX($B$2:$BY$77,B120,B121)</f>
-        <v>667.08320320631674</v>
+        <v>3100.4031995854989</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>42</v>
       </c>
       <c r="B121" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C121" s="1" cm="1">
         <f t="array" ref="C121">INDEX($B$2:$BY$77,B121,B122)</f>
-        <v>3700</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>43</v>
       </c>
       <c r="B122" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C122" s="1" cm="1">
         <f t="array" ref="C122">INDEX($B$2:$BY$77,B122,B123)</f>
-        <v>715.89105316381767</v>
+        <v>1629.4394741750921</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>44</v>
       </c>
       <c r="B123" s="2">
-        <v>43</v>
+        <v>51.000000000000007</v>
       </c>
       <c r="C123" s="1" cm="1">
         <f t="array" ref="C123">INDEX($B$2:$BY$77,B123,B124)</f>
-        <v>3707.4249823833252</v>
+        <v>1053.1728253235549</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>45</v>
       </c>
       <c r="B124" s="2">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C124" s="1" cm="1">
         <f t="array" ref="C124">INDEX($B$2:$BY$77,B124,B125)</f>
-        <v>1192.6860441876561</v>
+        <v>715.89105316381767</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>46</v>
       </c>
       <c r="B125" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C125" s="1" cm="1">
         <f t="array" ref="C125">INDEX($B$2:$BY$77,B125,B126)</f>
-        <v>1432.6548781894401</v>
+        <v>4069.705149024926</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>47</v>
       </c>
       <c r="B126" s="2">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C126" s="1" cm="1">
         <f t="array" ref="C126">INDEX($B$2:$BY$77,B126,B127)</f>
-        <v>3031.913587159107</v>
+        <v>1900</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>48</v>
       </c>
       <c r="B127" s="2">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C127" s="1" cm="1">
         <f t="array" ref="C127">INDEX($B$2:$BY$77,B127,B128)</f>
-        <v>1118.0339887498949</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>49</v>
       </c>
       <c r="B128" s="2">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C128" s="1" cm="1">
         <f t="array" ref="C128">INDEX($B$2:$BY$77,B128,B129)</f>
-        <v>2926.1749776799061</v>
+        <v>3250</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>50</v>
       </c>
       <c r="B129" s="2">
-        <v>49</v>
+        <v>63.999999999999993</v>
       </c>
       <c r="C129" s="1" cm="1">
         <f t="array" ref="C129">INDEX($B$2:$BY$77,B129,B130)</f>
-        <v>700</v>
+        <v>667.08320320631674</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>51</v>
       </c>
       <c r="B130" s="2">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C130" s="1" cm="1">
         <f t="array" ref="C130">INDEX($B$2:$BY$77,B130,B131)</f>
-        <v>1368.89480969138</v>
+        <v>1511.6216457830969</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>52</v>
       </c>
       <c r="B131" s="2">
-        <v>51</v>
+        <v>61.999999999999993</v>
       </c>
       <c r="C131" s="1" cm="1">
         <f t="array" ref="C131">INDEX($B$2:$BY$77,B131,B132)</f>
-        <v>1115.0004484304029</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>53</v>
       </c>
       <c r="B132" s="2">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C132" s="1" cm="1">
         <f t="array" ref="C132">INDEX($B$2:$BY$77,B132,B133)</f>
-        <v>905.84380552057644</v>
+        <v>1746.424919657298</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>54</v>
       </c>
       <c r="B133" s="2">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C133" s="1" cm="1">
         <f t="array" ref="C133">INDEX($B$2:$BY$77,B133,B134)</f>
-        <v>583.09518948453001</v>
+        <v>522.01532544552754</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>55</v>
       </c>
       <c r="B134" s="2">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C134" s="1" cm="1">
         <f t="array" ref="C134">INDEX($B$2:$BY$77,B134,B135)</f>
-        <v>2000</v>
+        <v>1164.11683262463</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>56</v>
       </c>
       <c r="B135" s="2">
-        <v>55</v>
+        <v>57.999999999999993</v>
       </c>
       <c r="C135" s="1" cm="1">
         <f t="array" ref="C135">INDEX($B$2:$BY$77,B135,B136)</f>
-        <v>700</v>
+        <v>1118.0004472271021</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>57</v>
       </c>
       <c r="B136" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C136" s="1" cm="1">
         <f t="array" ref="C136">INDEX($B$2:$BY$77,B136,B137)</f>
         <v>1616.696941297286</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>58</v>
       </c>
       <c r="B137" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C137" s="1" cm="1">
         <f t="array" ref="C137">INDEX($B$2:$BY$77,B137,B138)</f>
-        <v>1118.0004472271021</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>59</v>
       </c>
       <c r="B138" s="2">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C138" s="1" cm="1">
         <f t="array" ref="C138">INDEX($B$2:$BY$77,B138,B139)</f>
-        <v>1164.11683262463</v>
+        <v>1363.8009385537171</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>60</v>
       </c>
       <c r="B139" s="2">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C139" s="1" cm="1">
         <f t="array" ref="C139">INDEX($B$2:$BY$77,B139,B140)</f>
-        <v>522.01532544552754</v>
+        <v>905.84380552057644</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>61</v>
       </c>
       <c r="B140" s="2">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C140" s="1" cm="1">
         <f t="array" ref="C140">INDEX($B$2:$BY$77,B140,B141)</f>
-        <v>1746.424919657298</v>
+        <v>583.09518948453001</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>62</v>
       </c>
       <c r="B141" s="2">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C141" s="1" cm="1">
         <f t="array" ref="C141">INDEX($B$2:$BY$77,B141,B142)</f>
-        <v>700</v>
+        <v>550</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>63</v>
       </c>
       <c r="B142" s="2">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C142" s="1" cm="1">
         <f t="array" ref="C142">INDEX($B$2:$BY$77,B142,B143)</f>
-        <v>1511.6216457830969</v>
+        <v>715.89105316381767</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>64</v>
       </c>
       <c r="B143" s="2">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C143" s="1" cm="1">
         <f t="array" ref="C143">INDEX($B$2:$BY$77,B143,B144)</f>
-        <v>667.08320320631674</v>
+        <v>3272.6455658992468</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>65</v>
       </c>
       <c r="B144" s="2">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C144" s="1" cm="1">
         <f t="array" ref="C144">INDEX($B$2:$BY$77,B144,B145)</f>
-        <v>3700</v>
+        <v>1913.2979381162779</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>66</v>
       </c>
       <c r="B145" s="2">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C145" s="1" cm="1">
         <f t="array" ref="C145">INDEX($B$2:$BY$77,B145,B146)</f>
-        <v>715.89105316381767</v>
+        <v>667.08320320631674</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>67</v>
       </c>
       <c r="B146" s="2">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="C146" s="1" cm="1">
         <f t="array" ref="C146">INDEX($B$2:$BY$77,B146,B147)</f>
-        <v>3707.4249823833252</v>
+        <v>1511.6216457830969</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>68</v>
       </c>
       <c r="B147" s="2">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="C147" s="1" cm="1">
         <f t="array" ref="C147">INDEX($B$2:$BY$77,B147,B148)</f>
-        <v>1192.6860441876561</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>69</v>
       </c>
       <c r="B148" s="2">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C148" s="1" cm="1">
         <f t="array" ref="C148">INDEX($B$2:$BY$77,B148,B149)</f>
-        <v>1432.6548781894401</v>
+        <v>1390.143877445784</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>70</v>
       </c>
       <c r="B149" s="2">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C149" s="1" cm="1">
         <f t="array" ref="C149">INDEX($B$2:$BY$77,B149,B150)</f>
-        <v>4964.8766349225634</v>
+        <v>522.01532544552754</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>71</v>
       </c>
       <c r="B150" s="2">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C150" s="1" cm="1">
         <f t="array" ref="C150">INDEX($B$2:$BY$77,B150,B151)</f>
-        <v>9200</v>
+        <v>2412.9254029082622</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>72</v>
       </c>
       <c r="B151" s="2">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C151" s="1" cm="1">
         <f t="array" ref="C151">INDEX($B$2:$BY$77,B151,B152)</f>
-        <v>1900</v>
+        <v>1616.696941297286</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>73</v>
       </c>
       <c r="B152" s="2">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="C152" s="1" cm="1">
         <f t="array" ref="C152">INDEX($B$2:$BY$77,B152,B153)</f>
-        <v>300</v>
+        <v>1952.562418976664</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>74</v>
       </c>
       <c r="B153" s="2">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="C153" s="1" cm="1">
         <f t="array" ref="C153">INDEX($B$2:$BY$77,B153,B154)</f>
-        <v>19600</v>
+        <v>715.89105316381767</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>75</v>
       </c>
       <c r="B154" s="2">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="C154" s="1" cm="1">
         <f t="array" ref="C154">INDEX($B$2:$BY$77,B154,B155)</f>
-        <v>11100</v>
+        <v>550</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>76</v>
       </c>
       <c r="B155" s="2">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="C155" s="1" cm="1">
         <f t="array" ref="C155">INDEX($B$2:$BY$77,B155,B80)</f>
-        <v>3605.551275463989</v>
+        <v>583.09518948453001</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B156" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C156" s="1">
         <f>SUM(C80:C155)</f>
-        <v>156796.21835314916</v>
+        <v>118893.59439156638</v>
       </c>
     </row>
   </sheetData>
@@ -19368,18 +19368,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19497,18 +19497,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D7DFD2-2019-4F6F-832B-B10005936C21}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F3DE5B1-E60C-4E60-8EA0-7E4344374C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F3DE5B1-E60C-4E60-8EA0-7E4344374C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8D7DFD2-2019-4F6F-832B-B10005936C21}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>